<commit_message>
sim 2020 single sampling
</commit_message>
<xml_diff>
--- a/Result_files/V3_Bids_2020-01-13_2020-01-19.xlsx
+++ b/Result_files/V3_Bids_2020-01-13_2020-01-19.xlsx
@@ -557,10 +557,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>28.59199999999993</v>
+        <v>46.958</v>
       </c>
       <c r="J2" t="n">
-        <v>372.3124277387512</v>
+        <v>372.3124277387467</v>
       </c>
       <c r="K2" t="n">
         <v>33.99998</v>
@@ -598,7 +598,7 @@
         <v>148.96</v>
       </c>
       <c r="D3" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0.13</v>
@@ -616,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>281.0280277590296</v>
+        <v>281.0280277590306</v>
       </c>
       <c r="K3" t="n">
         <v>32.279999</v>
@@ -654,7 +654,7 @@
         <v>148.96</v>
       </c>
       <c r="D4" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
         <v>0.13</v>
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>2617.491670760711</v>
+        <v>277.3327307607113</v>
       </c>
       <c r="K4" t="n">
         <v>31.18</v>
@@ -710,7 +710,7 @@
         <v>148.96</v>
       </c>
       <c r="D5" t="n">
-        <v>47.8</v>
+        <v>42.2</v>
       </c>
       <c r="E5" t="n">
         <v>0.13</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>2534.97801977793</v>
+        <v>1492.630003691675</v>
       </c>
       <c r="K5" t="n">
         <v>30.1</v>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>2517.059296856684</v>
+        <v>2517.701239433797</v>
       </c>
       <c r="K6" t="n">
         <v>29.959999</v>
@@ -837,10 +837,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>25.675</v>
+        <v>25.33800000000001</v>
       </c>
       <c r="J7" t="n">
-        <v>1249.283229466323</v>
+        <v>937.5587463516456</v>
       </c>
       <c r="K7" t="n">
         <v>29.879999</v>
@@ -884,19 +884,19 @@
         <v>0.27</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="G8" t="n">
         <v>9.185999999999979</v>
       </c>
       <c r="H8" t="n">
-        <v>47.8</v>
+        <v>33.2</v>
       </c>
       <c r="I8" t="n">
         <v>7.425999999999988</v>
       </c>
       <c r="J8" t="n">
-        <v>-81.61734190178213</v>
+        <v>-553.7602109599987</v>
       </c>
       <c r="K8" t="n">
         <v>30.379999</v>
@@ -940,19 +940,19 @@
         <v>0.4</v>
       </c>
       <c r="F9" t="n">
-        <v>47.8</v>
+        <v>29.2</v>
       </c>
       <c r="G9" t="n">
         <v>7.699000000000012</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>18.6</v>
       </c>
       <c r="I9" t="n">
-        <v>6.288999999999975</v>
+        <v>6.270999999999901</v>
       </c>
       <c r="J9" t="n">
-        <v>2280.009424488325</v>
+        <v>-507.5675915516083</v>
       </c>
       <c r="K9" t="n">
         <v>31.15</v>
@@ -996,19 +996,19 @@
         <v>0.4</v>
       </c>
       <c r="F10" t="n">
-        <v>1.7</v>
+        <v>42.3</v>
       </c>
       <c r="G10" t="n">
         <v>7.699000000000012</v>
       </c>
       <c r="H10" t="n">
-        <v>46.1</v>
+        <v>5.5</v>
       </c>
       <c r="I10" t="n">
         <v>6.270999999999901</v>
       </c>
       <c r="J10" t="n">
-        <v>-472.8546411533842</v>
+        <v>-523.4585136300021</v>
       </c>
       <c r="K10" t="n">
         <v>32.9</v>
@@ -1046,7 +1046,7 @@
         <v>148.96</v>
       </c>
       <c r="D11" t="n">
-        <v>10.5</v>
+        <v>47.8</v>
       </c>
       <c r="E11" t="n">
         <v>0.4</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>-160.1824836771713</v>
+        <v>-841.5486720128647</v>
       </c>
       <c r="K11" t="n">
         <v>31.18</v>
@@ -1102,7 +1102,7 @@
         <v>148.96</v>
       </c>
       <c r="D12" t="n">
-        <v>13.5</v>
+        <v>47.8</v>
       </c>
       <c r="E12" t="n">
         <v>0.4</v>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>-161.3824804728733</v>
+        <v>-2415.183906850936</v>
       </c>
       <c r="K12" t="n">
         <v>31.6</v>
@@ -1158,7 +1158,7 @@
         <v>148.96</v>
       </c>
       <c r="D13" t="n">
-        <v>7.100000000000001</v>
+        <v>47.8</v>
       </c>
       <c r="E13" t="n">
         <v>0.4</v>
@@ -1176,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>-158.1405619992274</v>
+        <v>-3191.79011008622</v>
       </c>
       <c r="K13" t="n">
         <v>31.549999</v>
@@ -1214,7 +1214,7 @@
         <v>148.96</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>47.8</v>
       </c>
       <c r="E14" t="n">
         <v>0.4</v>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>-158.3822540000002</v>
+        <v>-3082.455801218119</v>
       </c>
       <c r="K14" t="n">
         <v>31.219999</v>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>-33.53667364924099</v>
+        <v>-1475.910679456807</v>
       </c>
       <c r="K15" t="n">
         <v>30.93</v>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>213.5635872558525</v>
+        <v>-680.6041882630356</v>
       </c>
       <c r="K16" t="n">
         <v>30.67</v>
@@ -1397,10 +1397,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>6.142</v>
+        <v>6.123999999999992</v>
       </c>
       <c r="J17" t="n">
-        <v>2214.006118216523</v>
+        <v>-357.8521756769059</v>
       </c>
       <c r="K17" t="n">
         <v>30.790001</v>
@@ -1453,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>6.142</v>
+        <v>6.123999999999992</v>
       </c>
       <c r="J18" t="n">
-        <v>2225.420383903559</v>
+        <v>-478.0792757757367</v>
       </c>
       <c r="K18" t="n">
         <v>31.16</v>
@@ -1509,10 +1509,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>6.142</v>
+        <v>6.123999999999992</v>
       </c>
       <c r="J19" t="n">
-        <v>2229.898041773221</v>
+        <v>1113.349998060077</v>
       </c>
       <c r="K19" t="n">
         <v>31.530001</v>
@@ -1556,19 +1556,19 @@
         <v>0.4</v>
       </c>
       <c r="F20" t="n">
-        <v>47.8</v>
+        <v>6.2</v>
       </c>
       <c r="G20" t="n">
         <v>6.88900000000001</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>41.6</v>
       </c>
       <c r="I20" t="n">
-        <v>6.659</v>
+        <v>6.125</v>
       </c>
       <c r="J20" t="n">
-        <v>2271.975483526922</v>
+        <v>-463.5114346796655</v>
       </c>
       <c r="K20" t="n">
         <v>31.1</v>
@@ -1612,19 +1612,19 @@
         <v>0.4</v>
       </c>
       <c r="F21" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>6.88900000000001</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I21" t="n">
-        <v>6.659</v>
+        <v>6.125</v>
       </c>
       <c r="J21" t="n">
-        <v>2247.775635622832</v>
+        <v>-37.02964841532381</v>
       </c>
       <c r="K21" t="n">
         <v>30.42</v>
@@ -1665,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1299999999996544</v>
+        <v>0.27</v>
       </c>
       <c r="F22" t="n">
         <v>47.8</v>
@@ -1677,10 +1677,10 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>6.659</v>
+        <v>6.143</v>
       </c>
       <c r="J22" t="n">
-        <v>2230.445447685434</v>
+        <v>2228.336086393475</v>
       </c>
       <c r="K22" t="n">
         <v>29.870001</v>
@@ -1724,19 +1724,19 @@
         <v>0.13</v>
       </c>
       <c r="F23" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>10.47399999999999</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I23" t="n">
-        <v>9.870999999999999</v>
+        <v>9.842999999999904</v>
       </c>
       <c r="J23" t="n">
-        <v>2076.44597120886</v>
+        <v>-247.4043226260678</v>
       </c>
       <c r="K23" t="n">
         <v>29.610001</v>
@@ -1780,19 +1780,19 @@
         <v>0.13</v>
       </c>
       <c r="F24" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
         <v>12.53899999999999</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I24" t="n">
-        <v>13.265</v>
+        <v>12.113</v>
       </c>
       <c r="J24" t="n">
-        <v>1960.505495565185</v>
+        <v>-326.6637395051068</v>
       </c>
       <c r="K24" t="n">
         <v>29.459999</v>
@@ -1845,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>25.513</v>
+        <v>25.45199999999999</v>
       </c>
       <c r="J25" t="n">
-        <v>1113.791422684677</v>
+        <v>1114.387254850684</v>
       </c>
       <c r="K25" t="n">
         <v>26.68</v>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>48.70299999999999</v>
+        <v>48.703</v>
       </c>
       <c r="H26" t="n">
         <v>47.8</v>
@@ -1904,7 +1904,7 @@
         <v>26.33599999999996</v>
       </c>
       <c r="J26" t="n">
-        <v>-1757.559049155185</v>
+        <v>-1757.559049155199</v>
       </c>
       <c r="K26" t="n">
         <v>29.16</v>
@@ -1942,7 +1942,7 @@
         <v>144</v>
       </c>
       <c r="D27" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E27" t="n">
         <v>0.13</v>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>282.5689349791241</v>
+        <v>282.5689349791131</v>
       </c>
       <c r="K27" t="n">
         <v>29</v>
@@ -1998,7 +1998,7 @@
         <v>144</v>
       </c>
       <c r="D28" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E28" t="n">
         <v>0.13</v>
@@ -2016,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>281.4332360318701</v>
+        <v>281.4332360318597</v>
       </c>
       <c r="K28" t="n">
         <v>29.8</v>
@@ -2054,7 +2054,7 @@
         <v>144</v>
       </c>
       <c r="D29" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E29" t="n">
         <v>0.13</v>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>2568.103459420238</v>
+        <v>271.1640183638562</v>
       </c>
       <c r="K29" t="n">
         <v>27.719999</v>
@@ -2110,7 +2110,7 @@
         <v>144</v>
       </c>
       <c r="D30" t="n">
-        <v>47.8</v>
+        <v>32.3</v>
       </c>
       <c r="E30" t="n">
         <v>0.13</v>
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>2548.460385894242</v>
+        <v>694.738709730302</v>
       </c>
       <c r="K30" t="n">
         <v>27.30001</v>
@@ -2172,19 +2172,19 @@
         <v>0.13</v>
       </c>
       <c r="F31" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>19.56099999999998</v>
+        <v>26.928</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I31" t="n">
         <v>17.59999999999997</v>
       </c>
       <c r="J31" t="n">
-        <v>1408.36371789076</v>
+        <v>-1143.264295211623</v>
       </c>
       <c r="K31" t="n">
         <v>27.620001</v>
@@ -2225,22 +2225,22 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.2699999999999818</v>
+        <v>0.4</v>
       </c>
       <c r="F32" t="n">
-        <v>47.8</v>
+        <v>31.2</v>
       </c>
       <c r="G32" t="n">
         <v>8.5</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>16.6</v>
       </c>
       <c r="I32" t="n">
         <v>6.802999999999997</v>
       </c>
       <c r="J32" t="n">
-        <v>2259.351337474794</v>
+        <v>-561.0130114800005</v>
       </c>
       <c r="K32" t="n">
         <v>33.18</v>
@@ -2296,7 +2296,7 @@
         <v>6.289</v>
       </c>
       <c r="J33" t="n">
-        <v>2295.798337460878</v>
+        <v>-895.546256430479</v>
       </c>
       <c r="K33" t="n">
         <v>34.209999</v>
@@ -2340,19 +2340,19 @@
         <v>0.4</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="G34" t="n">
-        <v>7.699</v>
+        <v>6.947000000000003</v>
       </c>
       <c r="H34" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>6.270999999999901</v>
+        <v>6.289</v>
       </c>
       <c r="J34" t="n">
-        <v>-74.40705461654881</v>
+        <v>-1365.825782091173</v>
       </c>
       <c r="K34" t="n">
         <v>35.75</v>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>130.2224118464034</v>
+        <v>-1320.717259729347</v>
       </c>
       <c r="K35" t="n">
         <v>32.52</v>
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>-20.83453200794516</v>
+        <v>-3297.292580530052</v>
       </c>
       <c r="K36" t="n">
         <v>32.9998</v>
@@ -2502,7 +2502,7 @@
         <v>144</v>
       </c>
       <c r="D37" t="n">
-        <v>47.7</v>
+        <v>47.8</v>
       </c>
       <c r="E37" t="n">
         <v>0.4</v>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1525.639773706743</v>
+        <v>-2930.839572818013</v>
       </c>
       <c r="K37" t="n">
         <v>31.23</v>
@@ -2558,7 +2558,7 @@
         <v>144</v>
       </c>
       <c r="D38" t="n">
-        <v>31.6</v>
+        <v>47.8</v>
       </c>
       <c r="E38" t="n">
         <v>0.4</v>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>-164.6799818527151</v>
+        <v>-4122.798526284968</v>
       </c>
       <c r="K38" t="n">
         <v>31.190001</v>
@@ -2614,7 +2614,7 @@
         <v>144</v>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
+        <v>47.8</v>
       </c>
       <c r="E39" t="n">
         <v>0.4</v>
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>-153.8822977919447</v>
+        <v>-2873.644626672474</v>
       </c>
       <c r="K39" t="n">
         <v>31.8</v>
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>671.6769506384054</v>
+        <v>-1780.489567256649</v>
       </c>
       <c r="K40" t="n">
         <v>31.209999</v>
@@ -2732,19 +2732,19 @@
         <v>0.4</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="G41" t="n">
-        <v>8.131</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H41" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>6.135000000000003</v>
       </c>
       <c r="J41" t="n">
-        <v>64.62047905258373</v>
+        <v>-764.381351337482</v>
       </c>
       <c r="K41" t="n">
         <v>31.299999</v>
@@ -2788,19 +2788,19 @@
         <v>0.4</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>34.1</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H42" t="n">
-        <v>47.8</v>
+        <v>13.7</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>6.123999999999994</v>
       </c>
       <c r="J42" t="n">
-        <v>69.0673605225421</v>
+        <v>-364.5938147500009</v>
       </c>
       <c r="K42" t="n">
         <v>33.580002</v>
@@ -2844,19 +2844,19 @@
         <v>0.4</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="G43" t="n">
-        <v>7.837</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H43" t="n">
-        <v>47.8</v>
+        <v>28.1</v>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>6.123999999999991</v>
       </c>
       <c r="J43" t="n">
-        <v>72.31816405236677</v>
+        <v>-369.334085950012</v>
       </c>
       <c r="K43" t="n">
         <v>34.49999</v>
@@ -2900,19 +2900,19 @@
         <v>0.4</v>
       </c>
       <c r="F44" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>6.88900000000001</v>
+        <v>7.323</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I44" t="n">
-        <v>6.143</v>
+        <v>6.125</v>
       </c>
       <c r="J44" t="n">
-        <v>2327.555958134345</v>
+        <v>-418.8552922198252</v>
       </c>
       <c r="K44" t="n">
         <v>31.309999</v>
@@ -2956,19 +2956,19 @@
         <v>0.4</v>
       </c>
       <c r="F45" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>6.88900000000001</v>
+        <v>7.323</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I45" t="n">
-        <v>6.304</v>
+        <v>6.125</v>
       </c>
       <c r="J45" t="n">
-        <v>2307.284988517304</v>
+        <v>-23.76784054604693</v>
       </c>
       <c r="K45" t="n">
         <v>30.950001</v>
@@ -3009,22 +3009,22 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1299999999996544</v>
+        <v>0.27</v>
       </c>
       <c r="F46" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>6.88900000000001</v>
+        <v>7.323</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I46" t="n">
-        <v>6.304</v>
+        <v>6.125</v>
       </c>
       <c r="J46" t="n">
-        <v>2291.327793754557</v>
+        <v>-14.85977453205849</v>
       </c>
       <c r="K46" t="n">
         <v>30.58</v>
@@ -3077,10 +3077,10 @@
         <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>11.005</v>
+        <v>12.719</v>
       </c>
       <c r="J47" t="n">
-        <v>2000.914952106548</v>
+        <v>2000.914952106535</v>
       </c>
       <c r="K47" t="n">
         <v>30.280001</v>
@@ -3133,10 +3133,10 @@
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>13.129</v>
+        <v>12.137</v>
       </c>
       <c r="J48" t="n">
-        <v>1919.001214807542</v>
+        <v>1916.903882863244</v>
       </c>
       <c r="K48" t="n">
         <v>29.459999</v>
@@ -3192,7 +3192,7 @@
         <v>14.89400000000001</v>
       </c>
       <c r="J49" t="n">
-        <v>1407.520530863874</v>
+        <v>1408.157206562968</v>
       </c>
       <c r="K49" t="n">
         <v>29.7</v>
@@ -3236,19 +3236,19 @@
         <v>0.13</v>
       </c>
       <c r="F50" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G50" t="n">
         <v>47.51799999999997</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I50" t="n">
-        <v>47.051</v>
+        <v>46.95799999999991</v>
       </c>
       <c r="J50" t="n">
-        <v>315.6202559140667</v>
+        <v>-1987.962196206585</v>
       </c>
       <c r="K50" t="n">
         <v>30.780001</v>
@@ -3286,7 +3286,7 @@
         <v>144</v>
       </c>
       <c r="D51" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E51" t="n">
         <v>0.13</v>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>2602.166710871908</v>
+        <v>276.480330501512</v>
       </c>
       <c r="K51" t="n">
         <v>30.639999</v>
@@ -3342,7 +3342,7 @@
         <v>144</v>
       </c>
       <c r="D52" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E52" t="n">
         <v>0.13</v>
@@ -3360,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>2609.692456394351</v>
+        <v>277.8109822735154</v>
       </c>
       <c r="K52" t="n">
         <v>30.43</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>2523.432983695548</v>
+        <v>2524.075924050169</v>
       </c>
       <c r="K53" t="n">
         <v>28.790001</v>
@@ -3472,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>2500.843454414431</v>
+        <v>2501.480982377348</v>
       </c>
       <c r="K54" t="n">
         <v>28.42</v>
@@ -3525,10 +3525,10 @@
         <v>0</v>
       </c>
       <c r="I55" t="n">
-        <v>27.116</v>
+        <v>25.675</v>
       </c>
       <c r="J55" t="n">
-        <v>1207.744151888713</v>
+        <v>1091.24257040246</v>
       </c>
       <c r="K55" t="n">
         <v>28.75</v>
@@ -3572,19 +3572,19 @@
         <v>0.27</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="G56" t="n">
         <v>9.185999999999979</v>
       </c>
       <c r="H56" t="n">
-        <v>47.8</v>
+        <v>43.2</v>
       </c>
       <c r="I56" t="n">
         <v>8.082999999999913</v>
       </c>
       <c r="J56" t="n">
-        <v>-96.42869449368136</v>
+        <v>-551.7451644662408</v>
       </c>
       <c r="K56" t="n">
         <v>33.380001</v>
@@ -3625,22 +3625,22 @@
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0.2699999999999818</v>
+        <v>0.4</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="G57" t="n">
         <v>7.699000000000012</v>
       </c>
       <c r="H57" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>6.270999999999901</v>
+        <v>6.288999999999979</v>
       </c>
       <c r="J57" t="n">
-        <v>-14.28906523669549</v>
+        <v>-678.2543808091644</v>
       </c>
       <c r="K57" t="n">
         <v>31.790001</v>
@@ -3681,22 +3681,22 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0.3899999999998727</v>
+        <v>0.4</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="G58" t="n">
         <v>7.699000000000012</v>
       </c>
       <c r="H58" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>6.270999999999901</v>
+        <v>6.288999999999979</v>
       </c>
       <c r="J58" t="n">
-        <v>-214.5785827300376</v>
+        <v>-1557.112937675758</v>
       </c>
       <c r="K58" t="n">
         <v>31.83</v>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>11.51728323456308</v>
+        <v>-1698.551820028121</v>
       </c>
       <c r="K59" t="n">
         <v>31.74</v>
@@ -3790,7 +3790,7 @@
         <v>144</v>
       </c>
       <c r="D60" t="n">
-        <v>47.8</v>
+        <v>41.90000000000001</v>
       </c>
       <c r="E60" t="n">
         <v>0.4</v>
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>-51.04762249065035</v>
+        <v>-170.5329600000017</v>
       </c>
       <c r="K60" t="n">
         <v>31.629999</v>
@@ -3864,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>-127.0045232798775</v>
+        <v>-2015.841227022939</v>
       </c>
       <c r="K61" t="n">
         <v>31.32</v>
@@ -3920,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>1.935310163826084</v>
+        <v>-1883.90465516362</v>
       </c>
       <c r="K62" t="n">
         <v>31.7</v>
@@ -3958,7 +3958,7 @@
         <v>144</v>
       </c>
       <c r="D63" t="n">
-        <v>5</v>
+        <v>43.5</v>
       </c>
       <c r="E63" t="n">
         <v>0.4</v>
@@ -3976,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>-14.38548218284246</v>
+        <v>-171.1729600000026</v>
       </c>
       <c r="K63" t="n">
         <v>31.59999</v>
@@ -4014,7 +4014,7 @@
         <v>144</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="E64" t="n">
         <v>0.3899999999998727</v>
@@ -4032,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>251.3423143752137</v>
+        <v>-262.484921916178</v>
       </c>
       <c r="K64" t="n">
         <v>31.7</v>
@@ -4073,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>0.3899999999998727</v>
+        <v>0.4</v>
       </c>
       <c r="F65" t="n">
         <v>47.8</v>
@@ -4085,10 +4085,10 @@
         <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>6.128</v>
+        <v>6.12800000000001</v>
       </c>
       <c r="J65" t="n">
-        <v>2257.891522931593</v>
+        <v>-2041.99885736612</v>
       </c>
       <c r="K65" t="n">
         <v>31.26</v>
@@ -4141,10 +4141,10 @@
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>6.142</v>
+        <v>6.12800000000001</v>
       </c>
       <c r="J66" t="n">
-        <v>2303.993687653243</v>
+        <v>-803.7386837826065</v>
       </c>
       <c r="K66" t="n">
         <v>31.41</v>
@@ -4188,19 +4188,19 @@
         <v>0.4</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>12.8</v>
       </c>
       <c r="G67" t="n">
         <v>7.836999999999989</v>
       </c>
       <c r="H67" t="n">
-        <v>47.8</v>
+        <v>35</v>
       </c>
       <c r="I67" t="n">
         <v>6.123999999999967</v>
       </c>
       <c r="J67" t="n">
-        <v>3.658159304697151</v>
+        <v>-478.8924686800105</v>
       </c>
       <c r="K67" t="n">
         <v>31.4</v>
@@ -4241,22 +4241,22 @@
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F68" t="n">
-        <v>47.8</v>
+        <v>1.3</v>
       </c>
       <c r="G68" t="n">
         <v>6.88900000000001</v>
       </c>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>46.5</v>
       </c>
       <c r="I68" t="n">
-        <v>6.143</v>
+        <v>6.125</v>
       </c>
       <c r="J68" t="n">
-        <v>2305.41868335368</v>
+        <v>-447.0833999391822</v>
       </c>
       <c r="K68" t="n">
         <v>31.1</v>
@@ -4297,22 +4297,22 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F69" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
         <v>6.88900000000001</v>
       </c>
       <c r="H69" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I69" t="n">
-        <v>6.129</v>
+        <v>6.125</v>
       </c>
       <c r="J69" t="n">
-        <v>2286.91493643055</v>
+        <v>-11.69249609712216</v>
       </c>
       <c r="K69" t="n">
         <v>30.75</v>
@@ -4353,22 +4353,22 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
       <c r="F70" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
         <v>6.88900000000001</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I70" t="n">
-        <v>6.143</v>
+        <v>6.125</v>
       </c>
       <c r="J70" t="n">
-        <v>2271.169508050019</v>
+        <v>-13.19127945519663</v>
       </c>
       <c r="K70" t="n">
         <v>30.469999</v>
@@ -4412,19 +4412,19 @@
         <v>0.13</v>
       </c>
       <c r="F71" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
         <v>10.47399999999999</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I71" t="n">
-        <v>9.870999999999999</v>
+        <v>9.842999999999904</v>
       </c>
       <c r="J71" t="n">
-        <v>2099.707091671571</v>
+        <v>-212.5104150578858</v>
       </c>
       <c r="K71" t="n">
         <v>30.1</v>
@@ -4468,19 +4468,19 @@
         <v>0.13</v>
       </c>
       <c r="F72" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
         <v>12.53899999999999</v>
       </c>
       <c r="H72" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I72" t="n">
-        <v>13.582</v>
+        <v>12.113</v>
       </c>
       <c r="J72" t="n">
-        <v>1969.921239171555</v>
+        <v>-323.8237074537411</v>
       </c>
       <c r="K72" t="n">
         <v>29.709999</v>
@@ -4536,7 +4536,7 @@
         <v>26.37</v>
       </c>
       <c r="J73" t="n">
-        <v>1242.619879945762</v>
+        <v>1243.246700995409</v>
       </c>
       <c r="K73" t="n">
         <v>24.99</v>
@@ -4589,10 +4589,10 @@
         <v>0</v>
       </c>
       <c r="I74" t="n">
-        <v>47.05100000000002</v>
+        <v>47.05100000000001</v>
       </c>
       <c r="J74" t="n">
-        <v>537.7336014600262</v>
+        <v>537.7336014600178</v>
       </c>
       <c r="K74" t="n">
         <v>33.99998</v>
@@ -4630,7 +4630,7 @@
         <v>144</v>
       </c>
       <c r="D75" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E75" t="n">
         <v>0.13</v>
@@ -4648,7 +4648,7 @@
         <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>280.6984689699194</v>
+        <v>280.6984689699098</v>
       </c>
       <c r="K75" t="n">
         <v>32.279999</v>
@@ -4686,7 +4686,7 @@
         <v>144</v>
       </c>
       <c r="D76" t="n">
-        <v>42.40000000000001</v>
+        <v>5</v>
       </c>
       <c r="E76" t="n">
         <v>0.13</v>
@@ -4704,7 +4704,7 @@
         <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>1515.64684918437</v>
+        <v>278.3522658333649</v>
       </c>
       <c r="K76" t="n">
         <v>31.18</v>
@@ -4742,7 +4742,7 @@
         <v>144</v>
       </c>
       <c r="D77" t="n">
-        <v>43.1</v>
+        <v>47.8</v>
       </c>
       <c r="E77" t="n">
         <v>0.13</v>
@@ -4760,7 +4760,7 @@
         <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>2492.261297424683</v>
+        <v>2029.717934485365</v>
       </c>
       <c r="K77" t="n">
         <v>30.1</v>
@@ -4816,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="J78" t="n">
-        <v>2516.17616369865</v>
+        <v>2516.817544222696</v>
       </c>
       <c r="K78" t="n">
         <v>29.959999</v>
@@ -4869,10 +4869,10 @@
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>27.116</v>
+        <v>25.675</v>
       </c>
       <c r="J79" t="n">
-        <v>1238.620754473918</v>
+        <v>1214.693357971275</v>
       </c>
       <c r="K79" t="n">
         <v>29.879999</v>
@@ -4913,22 +4913,22 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0.2699999999999818</v>
+        <v>0.4</v>
       </c>
       <c r="F80" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>8.5</v>
+        <v>9.186</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I80" t="n">
-        <v>8.773</v>
+        <v>6.802999999999997</v>
       </c>
       <c r="J80" t="n">
-        <v>2198.313720035393</v>
+        <v>-169.5724171966827</v>
       </c>
       <c r="K80" t="n">
         <v>30.379999</v>
@@ -4975,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>7.699</v>
+        <v>7.698999999999998</v>
       </c>
       <c r="H81" t="n">
         <v>47.8</v>
@@ -4984,7 +4984,7 @@
         <v>6.288999999999987</v>
       </c>
       <c r="J81" t="n">
-        <v>-64.83282315588843</v>
+        <v>-296.7596289476663</v>
       </c>
       <c r="K81" t="n">
         <v>31.15</v>
@@ -5028,19 +5028,19 @@
         <v>0.4</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>14.1</v>
       </c>
       <c r="G82" t="n">
         <v>6.947000000000003</v>
       </c>
       <c r="H82" t="n">
-        <v>47.7</v>
+        <v>33.7</v>
       </c>
       <c r="I82" t="n">
         <v>6.288999999999987</v>
       </c>
       <c r="J82" t="n">
-        <v>-483.636415318082</v>
+        <v>-516.7945094187638</v>
       </c>
       <c r="K82" t="n">
         <v>32.9</v>
@@ -5078,7 +5078,7 @@
         <v>144</v>
       </c>
       <c r="D83" t="n">
-        <v>9.600000000000001</v>
+        <v>45.6</v>
       </c>
       <c r="E83" t="n">
         <v>0.4</v>
@@ -5096,7 +5096,7 @@
         <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>-158.3599119775627</v>
+        <v>-172.3840414261081</v>
       </c>
       <c r="K83" t="n">
         <v>31.18</v>
@@ -5134,7 +5134,7 @@
         <v>144</v>
       </c>
       <c r="D84" t="n">
-        <v>28.8</v>
+        <v>47.8</v>
       </c>
       <c r="E84" t="n">
         <v>0.4</v>
@@ -5152,7 +5152,7 @@
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>-165.4580682167935</v>
+        <v>-248.9332763396449</v>
       </c>
       <c r="K84" t="n">
         <v>31.6</v>
@@ -5190,7 +5190,7 @@
         <v>144</v>
       </c>
       <c r="D85" t="n">
-        <v>32.8</v>
+        <v>47.8</v>
       </c>
       <c r="E85" t="n">
         <v>0.4</v>
@@ -5208,7 +5208,7 @@
         <v>0</v>
       </c>
       <c r="J85" t="n">
-        <v>-167.4404878450476</v>
+        <v>-353.8785725084851</v>
       </c>
       <c r="K85" t="n">
         <v>31.549999</v>
@@ -5246,7 +5246,7 @@
         <v>144</v>
       </c>
       <c r="D86" t="n">
-        <v>31.4</v>
+        <v>29.2</v>
       </c>
       <c r="E86" t="n">
         <v>0.4</v>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="J86" t="n">
-        <v>-166.4828132322818</v>
+        <v>-166.1995639999997</v>
       </c>
       <c r="K86" t="n">
         <v>31.219999</v>
@@ -5302,7 +5302,7 @@
         <v>144</v>
       </c>
       <c r="D87" t="n">
-        <v>10.5</v>
+        <v>41.90000000000001</v>
       </c>
       <c r="E87" t="n">
         <v>0.4</v>
@@ -5320,7 +5320,7 @@
         <v>0</v>
       </c>
       <c r="J87" t="n">
-        <v>-158.7195639999999</v>
+        <v>-171.2795640000023</v>
       </c>
       <c r="K87" t="n">
         <v>30.93</v>
@@ -5358,7 +5358,7 @@
         <v>144</v>
       </c>
       <c r="D88" t="n">
-        <v>11.6</v>
+        <v>47.8</v>
       </c>
       <c r="E88" t="n">
         <v>0.4</v>
@@ -5376,7 +5376,7 @@
         <v>0</v>
       </c>
       <c r="J88" t="n">
-        <v>271.3435600561888</v>
+        <v>-226.4099090168439</v>
       </c>
       <c r="K88" t="n">
         <v>30.67</v>
@@ -5423,16 +5423,16 @@
         <v>47.8</v>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
+        <v>7.836999999999989</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
       </c>
       <c r="I89" t="n">
-        <v>6.128000000000002</v>
+        <v>6.142</v>
       </c>
       <c r="J89" t="n">
-        <v>1674.271091756003</v>
+        <v>512.9343510520197</v>
       </c>
       <c r="K89" t="n">
         <v>30.790001</v>
@@ -5488,7 +5488,7 @@
         <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>1717.014294504641</v>
+        <v>1003.862680658491</v>
       </c>
       <c r="K90" t="n">
         <v>31.16</v>
@@ -5532,19 +5532,19 @@
         <v>0.4</v>
       </c>
       <c r="F91" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>0</v>
+        <v>7.837</v>
       </c>
       <c r="H91" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I91" t="n">
-        <v>0</v>
+        <v>6.128000000000013</v>
       </c>
       <c r="J91" t="n">
-        <v>1738.082610159026</v>
+        <v>-303.7278465937404</v>
       </c>
       <c r="K91" t="n">
         <v>31.530001</v>
@@ -5591,7 +5591,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>6.991</v>
+        <v>8.628</v>
       </c>
       <c r="H92" t="n">
         <v>47.8</v>
@@ -5600,7 +5600,7 @@
         <v>6.128999999999962</v>
       </c>
       <c r="J92" t="n">
-        <v>-17.31435557382869</v>
+        <v>-131.9972635074631</v>
       </c>
       <c r="K92" t="n">
         <v>31.1</v>
@@ -5644,19 +5644,19 @@
         <v>0.4</v>
       </c>
       <c r="F93" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>6.88900000000001</v>
+        <v>6.991</v>
       </c>
       <c r="H93" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I93" t="n">
-        <v>6.659</v>
+        <v>6.128999999999962</v>
       </c>
       <c r="J93" t="n">
-        <v>2272.444665522061</v>
+        <v>-21.79280756607461</v>
       </c>
       <c r="K93" t="n">
         <v>30.42</v>
@@ -5697,22 +5697,22 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0.1299999999996544</v>
+        <v>0.27</v>
       </c>
       <c r="F94" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>6.88900000000001</v>
+        <v>6.991</v>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I94" t="n">
-        <v>6.659</v>
+        <v>6.128999999999962</v>
       </c>
       <c r="J94" t="n">
-        <v>2249.44045054385</v>
+        <v>-25.65751248330496</v>
       </c>
       <c r="K94" t="n">
         <v>29.870001</v>
@@ -5756,19 +5756,19 @@
         <v>0.13</v>
       </c>
       <c r="F95" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>10.96600000000001</v>
+        <v>11.15899999999999</v>
       </c>
       <c r="H95" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I95" t="n">
-        <v>13.265</v>
+        <v>9.870999999999924</v>
       </c>
       <c r="J95" t="n">
-        <v>1987.174635956741</v>
+        <v>-291.8951850610603</v>
       </c>
       <c r="K95" t="n">
         <v>29.610001</v>
@@ -5821,10 +5821,10 @@
         <v>0</v>
       </c>
       <c r="I96" t="n">
-        <v>12.719</v>
+        <v>12.137</v>
       </c>
       <c r="J96" t="n">
-        <v>1896.077475393989</v>
+        <v>1894.003753964959</v>
       </c>
       <c r="K96" t="n">
         <v>29.459999</v>
@@ -5877,10 +5877,10 @@
         <v>0</v>
       </c>
       <c r="I97" t="n">
-        <v>16.286</v>
+        <v>25.51300000000001</v>
       </c>
       <c r="J97" t="n">
-        <v>1278.900283128693</v>
+        <v>1279.524167748083</v>
       </c>
       <c r="K97" t="n">
         <v>26.68</v>
@@ -5933,10 +5933,10 @@
         <v>0</v>
       </c>
       <c r="I98" t="n">
-        <v>28.59199999999993</v>
+        <v>32.096</v>
       </c>
       <c r="J98" t="n">
-        <v>573.0143834164329</v>
+        <v>573.014383416427</v>
       </c>
       <c r="K98" t="n">
         <v>29.16</v>
@@ -5974,7 +5974,7 @@
         <v>149</v>
       </c>
       <c r="D99" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E99" t="n">
         <v>0.13</v>
@@ -5992,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>922.5256446447221</v>
+        <v>275.5504927498162</v>
       </c>
       <c r="K99" t="n">
         <v>29</v>
@@ -6030,7 +6030,7 @@
         <v>149</v>
       </c>
       <c r="D100" t="n">
-        <v>30.6</v>
+        <v>5</v>
       </c>
       <c r="E100" t="n">
         <v>0.13</v>
@@ -6048,7 +6048,7 @@
         <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>1331.912115429809</v>
+        <v>275.0592859763416</v>
       </c>
       <c r="K100" t="n">
         <v>29.8</v>
@@ -6104,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="J101" t="n">
-        <v>2515.214538220473</v>
+        <v>2515.856154518034</v>
       </c>
       <c r="K101" t="n">
         <v>27.719999</v>
@@ -6160,7 +6160,7 @@
         <v>0</v>
       </c>
       <c r="J102" t="n">
-        <v>2497.552932808342</v>
+        <v>2498.19031743174</v>
       </c>
       <c r="K102" t="n">
         <v>27.30001</v>
@@ -6213,10 +6213,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="n">
-        <v>26.12</v>
+        <v>25.33799999999999</v>
       </c>
       <c r="J103" t="n">
-        <v>1332.067231441384</v>
+        <v>1281.527589270648</v>
       </c>
       <c r="K103" t="n">
         <v>27.620001</v>
@@ -6260,19 +6260,19 @@
         <v>0.27</v>
       </c>
       <c r="F104" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="G104" t="n">
-        <v>9.452999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="H104" t="n">
-        <v>47.8</v>
+        <v>45.1</v>
       </c>
       <c r="I104" t="n">
         <v>7.425999999999988</v>
       </c>
       <c r="J104" t="n">
-        <v>-145.089269140957</v>
+        <v>-592.5287897099997</v>
       </c>
       <c r="K104" t="n">
         <v>33.18</v>
@@ -6313,22 +6313,22 @@
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>0.2699999999999818</v>
+        <v>0.4</v>
       </c>
       <c r="F105" t="n">
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="G105" t="n">
-        <v>8.954000000000001</v>
+        <v>6.947000000000003</v>
       </c>
       <c r="H105" t="n">
-        <v>47.8</v>
+        <v>24.3</v>
       </c>
       <c r="I105" t="n">
         <v>6.270999999999901</v>
       </c>
       <c r="J105" t="n">
-        <v>-188.4538010228329</v>
+        <v>-547.9915238000003</v>
       </c>
       <c r="K105" t="n">
         <v>34.209999</v>
@@ -6369,22 +6369,22 @@
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>0.3899999999998727</v>
+        <v>0.4</v>
       </c>
       <c r="F106" t="n">
-        <v>5.9</v>
+        <v>46.2</v>
       </c>
       <c r="G106" t="n">
         <v>6.947000000000003</v>
       </c>
       <c r="H106" t="n">
-        <v>41.90000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="I106" t="n">
         <v>6.270999999999901</v>
       </c>
       <c r="J106" t="n">
-        <v>-554.5637052399998</v>
+        <v>-539.5149034200036</v>
       </c>
       <c r="K106" t="n">
         <v>35.75</v>
@@ -6422,7 +6422,7 @@
         <v>149</v>
       </c>
       <c r="D107" t="n">
-        <v>27.7</v>
+        <v>40.2</v>
       </c>
       <c r="E107" t="n">
         <v>0.4</v>
@@ -6440,7 +6440,7 @@
         <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>-167.5452299999996</v>
+        <v>-172.5452300000005</v>
       </c>
       <c r="K107" t="n">
         <v>32.52</v>
@@ -6478,7 +6478,7 @@
         <v>149</v>
       </c>
       <c r="D108" t="n">
-        <v>37</v>
+        <v>47.8</v>
       </c>
       <c r="E108" t="n">
         <v>0.4</v>
@@ -6496,7 +6496,7 @@
         <v>0</v>
       </c>
       <c r="J108" t="n">
-        <v>-171.2652299999998</v>
+        <v>-799.9798686531436</v>
       </c>
       <c r="K108" t="n">
         <v>32.9998</v>
@@ -6534,7 +6534,7 @@
         <v>149</v>
       </c>
       <c r="D109" t="n">
-        <v>41.8</v>
+        <v>47.8</v>
       </c>
       <c r="E109" t="n">
         <v>0.4</v>
@@ -6552,7 +6552,7 @@
         <v>0</v>
       </c>
       <c r="J109" t="n">
-        <v>-172.3438666878572</v>
+        <v>-908.9228013289219</v>
       </c>
       <c r="K109" t="n">
         <v>31.23</v>
@@ -6590,7 +6590,7 @@
         <v>149</v>
       </c>
       <c r="D110" t="n">
-        <v>33.3</v>
+        <v>28</v>
       </c>
       <c r="E110" t="n">
         <v>0.4</v>
@@ -6608,7 +6608,7 @@
         <v>0</v>
       </c>
       <c r="J110" t="n">
-        <v>-169.4520631717999</v>
+        <v>-167.4598957357885</v>
       </c>
       <c r="K110" t="n">
         <v>31.190001</v>
@@ -6646,7 +6646,7 @@
         <v>149</v>
       </c>
       <c r="D111" t="n">
-        <v>14.2</v>
+        <v>17.8</v>
       </c>
       <c r="E111" t="n">
         <v>0.4</v>
@@ -6664,7 +6664,7 @@
         <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>-162.1453477128923</v>
+        <v>-163.0910878586584</v>
       </c>
       <c r="K111" t="n">
         <v>31.8</v>
@@ -6702,7 +6702,7 @@
         <v>149</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>24.2</v>
       </c>
       <c r="E112" t="n">
         <v>0.3899999999998727</v>
@@ -6720,7 +6720,7 @@
         <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>-102.0786431807021</v>
+        <v>-166.054649399994</v>
       </c>
       <c r="K112" t="n">
         <v>31.209999</v>
@@ -6761,13 +6761,13 @@
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>0.3899999999998727</v>
+        <v>0.4</v>
       </c>
       <c r="F113" t="n">
         <v>47.8</v>
       </c>
       <c r="G113" t="n">
-        <v>0</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H113" t="n">
         <v>0</v>
@@ -6776,7 +6776,7 @@
         <v>6.124</v>
       </c>
       <c r="J113" t="n">
-        <v>1674.759721775105</v>
+        <v>134.1613106095918</v>
       </c>
       <c r="K113" t="n">
         <v>31.299999</v>
@@ -6823,7 +6823,7 @@
         <v>47.8</v>
       </c>
       <c r="G114" t="n">
-        <v>0</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H114" t="n">
         <v>0</v>
@@ -6832,7 +6832,7 @@
         <v>6.124</v>
       </c>
       <c r="J114" t="n">
-        <v>1727.707521834027</v>
+        <v>1104.010825973148</v>
       </c>
       <c r="K114" t="n">
         <v>33.580002</v>
@@ -6888,7 +6888,7 @@
         <v>6.124</v>
       </c>
       <c r="J115" t="n">
-        <v>1751.927884232044</v>
+        <v>1204.069530089575</v>
       </c>
       <c r="K115" t="n">
         <v>34.49999</v>
@@ -6929,7 +6929,7 @@
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F116" t="n">
         <v>0</v>
@@ -6944,7 +6944,7 @@
         <v>6.125</v>
       </c>
       <c r="J116" t="n">
-        <v>-55.55147240842251</v>
+        <v>-239.6600531817419</v>
       </c>
       <c r="K116" t="n">
         <v>31.309999</v>
@@ -6985,13 +6985,13 @@
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F117" t="n">
         <v>0</v>
       </c>
       <c r="G117" t="n">
-        <v>7.322999999999993</v>
+        <v>7.323</v>
       </c>
       <c r="H117" t="n">
         <v>47.8</v>
@@ -7000,7 +7000,7 @@
         <v>6.125</v>
       </c>
       <c r="J117" t="n">
-        <v>-59.71750184349735</v>
+        <v>-59.71750184351228</v>
       </c>
       <c r="K117" t="n">
         <v>30.950001</v>
@@ -7041,22 +7041,22 @@
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
       <c r="F118" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>6.88900000000001</v>
+        <v>7.323</v>
       </c>
       <c r="H118" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I118" t="n">
         <v>6.125</v>
       </c>
       <c r="J118" t="n">
-        <v>2235.88368351362</v>
+        <v>-63.40647212332055</v>
       </c>
       <c r="K118" t="n">
         <v>30.58</v>
@@ -7112,7 +7112,7 @@
         <v>9.842999999999904</v>
       </c>
       <c r="J119" t="n">
-        <v>-333.3136717274803</v>
+        <v>-335.4092204403341</v>
       </c>
       <c r="K119" t="n">
         <v>30.280001</v>
@@ -7156,19 +7156,19 @@
         <v>0.13</v>
       </c>
       <c r="F120" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>12.53899999999999</v>
+        <v>13.139</v>
       </c>
       <c r="H120" t="n">
-        <v>17.8</v>
+        <v>47.8</v>
       </c>
       <c r="I120" t="n">
         <v>12.113</v>
       </c>
       <c r="J120" t="n">
-        <v>1061.18118923399</v>
+        <v>-378.2316971949943</v>
       </c>
       <c r="K120" t="n">
         <v>29.459999</v>
@@ -7221,10 +7221,10 @@
         <v>0</v>
       </c>
       <c r="I121" t="n">
-        <v>25.452</v>
+        <v>18.555</v>
       </c>
       <c r="J121" t="n">
-        <v>1324.197863205941</v>
+        <v>1322.672520547489</v>
       </c>
       <c r="K121" t="n">
         <v>29.7</v>
@@ -7277,10 +7277,10 @@
         <v>0</v>
       </c>
       <c r="I122" t="n">
-        <v>50.635</v>
+        <v>46.95800000000001</v>
       </c>
       <c r="J122" t="n">
-        <v>98.28864611144074</v>
+        <v>98.90894909370711</v>
       </c>
       <c r="K122" t="n">
         <v>30.780001</v>
@@ -7336,7 +7336,7 @@
         <v>0</v>
       </c>
       <c r="J123" t="n">
-        <v>2391.411500700241</v>
+        <v>2392.023110107277</v>
       </c>
       <c r="K123" t="n">
         <v>30.639999</v>
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="J124" t="n">
-        <v>2367.638600009722</v>
+        <v>2368.244513492331</v>
       </c>
       <c r="K124" t="n">
         <v>30.43</v>
@@ -7448,7 +7448,7 @@
         <v>0</v>
       </c>
       <c r="J125" t="n">
-        <v>2307.200326063546</v>
+        <v>2307.791758694817</v>
       </c>
       <c r="K125" t="n">
         <v>28.790001</v>
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>2291.725750678646</v>
+        <v>2292.313475642397</v>
       </c>
       <c r="K126" t="n">
         <v>28.42</v>
@@ -7557,10 +7557,10 @@
         <v>0</v>
       </c>
       <c r="I127" t="n">
-        <v>27.142</v>
+        <v>25.338</v>
       </c>
       <c r="J127" t="n">
-        <v>1027.748775178685</v>
+        <v>876.739408460611</v>
       </c>
       <c r="K127" t="n">
         <v>28.75</v>
@@ -7601,7 +7601,7 @@
         <v>0</v>
       </c>
       <c r="E128" t="n">
-        <v>0.1299999999996544</v>
+        <v>0.27</v>
       </c>
       <c r="F128" t="n">
         <v>47.8</v>
@@ -7613,10 +7613,10 @@
         <v>0</v>
       </c>
       <c r="I128" t="n">
-        <v>8.093</v>
+        <v>8.083</v>
       </c>
       <c r="J128" t="n">
-        <v>1995.973101371886</v>
+        <v>1508.216963390206</v>
       </c>
       <c r="K128" t="n">
         <v>33.380001</v>
@@ -7669,10 +7669,10 @@
         <v>0</v>
       </c>
       <c r="I129" t="n">
-        <v>7.426</v>
+        <v>6.282</v>
       </c>
       <c r="J129" t="n">
-        <v>2084.339924194681</v>
+        <v>1771.314200656996</v>
       </c>
       <c r="K129" t="n">
         <v>31.790001</v>
@@ -7716,19 +7716,19 @@
         <v>0.4</v>
       </c>
       <c r="F130" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>6.947000000000003</v>
+        <v>8.000999999999999</v>
       </c>
       <c r="H130" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I130" t="n">
-        <v>7.426</v>
+        <v>6.270999999999901</v>
       </c>
       <c r="J130" t="n">
-        <v>1617.400612761239</v>
+        <v>-390.258014003577</v>
       </c>
       <c r="K130" t="n">
         <v>31.83</v>
@@ -7784,7 +7784,7 @@
         <v>0</v>
       </c>
       <c r="J131" t="n">
-        <v>1759.599452596537</v>
+        <v>-899.2385595368679</v>
       </c>
       <c r="K131" t="n">
         <v>31.74</v>
@@ -7840,7 +7840,7 @@
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>1000.042125191366</v>
+        <v>-2219.668007497949</v>
       </c>
       <c r="K132" t="n">
         <v>31.629999</v>
@@ -7878,7 +7878,7 @@
         <v>150</v>
       </c>
       <c r="D133" t="n">
-        <v>47.8</v>
+        <v>44.90000000000001</v>
       </c>
       <c r="E133" t="n">
         <v>0.4</v>
@@ -7896,7 +7896,7 @@
         <v>0</v>
       </c>
       <c r="J133" t="n">
-        <v>1236.786638434361</v>
+        <v>-172.9894520000005</v>
       </c>
       <c r="K133" t="n">
         <v>31.32</v>
@@ -7952,7 +7952,7 @@
         <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>1364.317651013624</v>
+        <v>-1742.602749670357</v>
       </c>
       <c r="K134" t="n">
         <v>31.7</v>
@@ -8008,7 +8008,7 @@
         <v>0</v>
       </c>
       <c r="J135" t="n">
-        <v>2154.139970626122</v>
+        <v>-2069.69639669162</v>
       </c>
       <c r="K135" t="n">
         <v>31.59999</v>
@@ -8046,7 +8046,7 @@
         <v>150</v>
       </c>
       <c r="D136" t="n">
-        <v>47.8</v>
+        <v>17.5</v>
       </c>
       <c r="E136" t="n">
         <v>0.4</v>
@@ -8064,7 +8064,7 @@
         <v>0</v>
       </c>
       <c r="J136" t="n">
-        <v>2352.667160426495</v>
+        <v>-162.0294520000008</v>
       </c>
       <c r="K136" t="n">
         <v>31.7</v>
@@ -8117,10 +8117,10 @@
         <v>0</v>
       </c>
       <c r="I137" t="n">
-        <v>6.135</v>
+        <v>6.123999999999986</v>
       </c>
       <c r="J137" t="n">
-        <v>2113.872687523729</v>
+        <v>-759.6634201813907</v>
       </c>
       <c r="K137" t="n">
         <v>31.26</v>
@@ -8173,10 +8173,10 @@
         <v>0</v>
       </c>
       <c r="I138" t="n">
-        <v>6.124</v>
+        <v>6.123999999999986</v>
       </c>
       <c r="J138" t="n">
-        <v>2156.029487386099</v>
+        <v>795.5720171853933</v>
       </c>
       <c r="K138" t="n">
         <v>31.41</v>
@@ -8217,7 +8217,7 @@
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F139" t="n">
         <v>47.8</v>
@@ -8229,10 +8229,10 @@
         <v>0</v>
       </c>
       <c r="I139" t="n">
-        <v>6.135</v>
+        <v>6.123999999999986</v>
       </c>
       <c r="J139" t="n">
-        <v>2188.005926899946</v>
+        <v>547.2525398248903</v>
       </c>
       <c r="K139" t="n">
         <v>31.4</v>
@@ -8273,22 +8273,22 @@
         <v>0</v>
       </c>
       <c r="E140" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F140" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>6.88900000000001</v>
+        <v>9.378</v>
       </c>
       <c r="H140" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I140" t="n">
-        <v>6.659</v>
+        <v>6.125</v>
       </c>
       <c r="J140" t="n">
-        <v>2200.236051401469</v>
+        <v>-207.8467727304169</v>
       </c>
       <c r="K140" t="n">
         <v>31.1</v>
@@ -8329,22 +8329,22 @@
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>0.3999999999996362</v>
+        <v>0.54</v>
       </c>
       <c r="F141" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G141" t="n">
-        <v>6.88900000000001</v>
+        <v>9.378</v>
       </c>
       <c r="H141" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I141" t="n">
-        <v>6.659</v>
+        <v>6.125</v>
       </c>
       <c r="J141" t="n">
-        <v>2175.459509935618</v>
+        <v>-35.55955305379222</v>
       </c>
       <c r="K141" t="n">
         <v>30.75</v>
@@ -8385,22 +8385,22 @@
         <v>0</v>
       </c>
       <c r="E142" t="n">
-        <v>0.1299999999996544</v>
+        <v>0.27</v>
       </c>
       <c r="F142" t="n">
-        <v>47.8</v>
+        <v>14.3</v>
       </c>
       <c r="G142" t="n">
         <v>6.88900000000001</v>
       </c>
       <c r="H142" t="n">
-        <v>0</v>
+        <v>33.5</v>
       </c>
       <c r="I142" t="n">
-        <v>6.659</v>
+        <v>6.125</v>
       </c>
       <c r="J142" t="n">
-        <v>2151.077621633582</v>
+        <v>615.1075883493588</v>
       </c>
       <c r="K142" t="n">
         <v>30.469999</v>
@@ -8447,7 +8447,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>10.966</v>
+        <v>11.159</v>
       </c>
       <c r="H143" t="n">
         <v>47.8</v>
@@ -8456,7 +8456,7 @@
         <v>9.842999999999904</v>
       </c>
       <c r="J143" t="n">
-        <v>-291.1661372285729</v>
+        <v>-294.047324081178</v>
       </c>
       <c r="K143" t="n">
         <v>30.1</v>
@@ -8500,19 +8500,19 @@
         <v>0.13</v>
       </c>
       <c r="F144" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>12.53899999999999</v>
+        <v>13.139</v>
       </c>
       <c r="H144" t="n">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="I144" t="n">
-        <v>13.265</v>
+        <v>12.113</v>
       </c>
       <c r="J144" t="n">
-        <v>1869.806998070696</v>
+        <v>-353.7252238571727</v>
       </c>
       <c r="K144" t="n">
         <v>29.709999</v>
@@ -8565,10 +8565,10 @@
         <v>0</v>
       </c>
       <c r="I145" t="n">
-        <v>25.942</v>
+        <v>25.45200000000001</v>
       </c>
       <c r="J145" t="n">
-        <v>1165.6373417718</v>
+        <v>1166.246468004644</v>
       </c>
       <c r="K145" t="n">
         <v>24.99</v>
@@ -8624,7 +8624,7 @@
         <v>28.59199999999993</v>
       </c>
       <c r="J146" t="n">
-        <v>597.8590454267941</v>
+        <v>597.8590454267791</v>
       </c>
       <c r="K146" t="n">
         <v>30.780001</v>
@@ -8662,7 +8662,7 @@
         <v>148.96</v>
       </c>
       <c r="D147" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E147" t="n">
         <v>0.13</v>
@@ -8680,7 +8680,7 @@
         <v>0</v>
       </c>
       <c r="J147" t="n">
-        <v>284.9132723888475</v>
+        <v>284.9132723888357</v>
       </c>
       <c r="K147" t="n">
         <v>30.639999</v>
@@ -8718,7 +8718,7 @@
         <v>148.96</v>
       </c>
       <c r="D148" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="E148" t="n">
         <v>0.13</v>
@@ -8736,7 +8736,7 @@
         <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>280.0401467224876</v>
+        <v>280.0401467224751</v>
       </c>
       <c r="K148" t="n">
         <v>30.43</v>
@@ -8774,7 +8774,7 @@
         <v>148.96</v>
       </c>
       <c r="D149" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="E149" t="n">
         <v>0.13</v>
@@ -8792,7 +8792,7 @@
         <v>0</v>
       </c>
       <c r="J149" t="n">
-        <v>431.1546004176171</v>
+        <v>267.7712121141292</v>
       </c>
       <c r="K149" t="n">
         <v>28.790001</v>
@@ -8830,7 +8830,7 @@
         <v>148.96</v>
       </c>
       <c r="D150" t="n">
-        <v>47.8</v>
+        <v>5</v>
       </c>
       <c r="E150" t="n">
         <v>0.13</v>
@@ -8848,7 +8848,7 @@
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>1496.618984513896</v>
+        <v>265.6180340881157</v>
       </c>
       <c r="K150" t="n">
         <v>28.42</v>
@@ -8895,7 +8895,7 @@
         <v>0</v>
       </c>
       <c r="G151" t="n">
-        <v>27.911</v>
+        <v>26.31600000000001</v>
       </c>
       <c r="H151" t="n">
         <v>47.8</v>
@@ -8904,7 +8904,7 @@
         <v>18.05899999999991</v>
       </c>
       <c r="J151" t="n">
-        <v>-868.3558491711627</v>
+        <v>-1133.622264635602</v>
       </c>
       <c r="K151" t="n">
         <v>28.75</v>
@@ -8948,19 +8948,19 @@
         <v>0.27</v>
       </c>
       <c r="F152" t="n">
-        <v>0</v>
+        <v>26.5</v>
       </c>
       <c r="G152" t="n">
-        <v>9.452999999999999</v>
+        <v>0</v>
       </c>
       <c r="H152" t="n">
-        <v>47.8</v>
+        <v>21.3</v>
       </c>
       <c r="I152" t="n">
         <v>7.425999999999988</v>
       </c>
       <c r="J152" t="n">
-        <v>-146.2148998773517</v>
+        <v>-554.45203123</v>
       </c>
       <c r="K152" t="n">
         <v>33.380001</v>
@@ -9004,19 +9004,19 @@
         <v>0.4</v>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
+        <v>28.4</v>
       </c>
       <c r="G153" t="n">
-        <v>13.875</v>
+        <v>7.699000000000012</v>
       </c>
       <c r="H153" t="n">
-        <v>47.8</v>
+        <v>19.4</v>
       </c>
       <c r="I153" t="n">
         <v>6.270999999999901</v>
       </c>
       <c r="J153" t="n">
-        <v>-169.6603630848049</v>
+        <v>-507.139932440001</v>
       </c>
       <c r="K153" t="n">
         <v>31.790001</v>
@@ -9060,19 +9060,19 @@
         <v>0.4</v>
       </c>
       <c r="F154" t="n">
-        <v>9.700000000000001</v>
+        <v>43.8</v>
       </c>
       <c r="G154" t="n">
-        <v>0</v>
+        <v>7.699000000000012</v>
       </c>
       <c r="H154" t="n">
-        <v>38.1</v>
+        <v>4</v>
       </c>
       <c r="I154" t="n">
         <v>6.270999999999901</v>
       </c>
       <c r="J154" t="n">
-        <v>-525.31887003</v>
+        <v>-492.1690426600072</v>
       </c>
       <c r="K154" t="n">
         <v>31.83</v>
@@ -9110,7 +9110,7 @@
         <v>148.96</v>
       </c>
       <c r="D155" t="n">
-        <v>26.2</v>
+        <v>47.8</v>
       </c>
       <c r="E155" t="n">
         <v>0.4</v>
@@ -9128,7 +9128,7 @@
         <v>0</v>
       </c>
       <c r="J155" t="n">
-        <v>-165.0961264127226</v>
+        <v>-646.767136150271</v>
       </c>
       <c r="K155" t="n">
         <v>31.74</v>
@@ -9166,7 +9166,7 @@
         <v>148.96</v>
       </c>
       <c r="D156" t="n">
-        <v>39.40000000000001</v>
+        <v>47.8</v>
       </c>
       <c r="E156" t="n">
         <v>0.4</v>
@@ -9184,7 +9184,7 @@
         <v>0</v>
       </c>
       <c r="J156" t="n">
-        <v>-170.3761268072161</v>
+        <v>-3294.412266797672</v>
       </c>
       <c r="K156" t="n">
         <v>31.629999</v>
@@ -9222,7 +9222,7 @@
         <v>148.96</v>
       </c>
       <c r="D157" t="n">
-        <v>42.5</v>
+        <v>47.8</v>
       </c>
       <c r="E157" t="n">
         <v>0.4</v>
@@ -9240,7 +9240,7 @@
         <v>0</v>
       </c>
       <c r="J157" t="n">
-        <v>-171.6160080000003</v>
+        <v>-1103.362410115707</v>
       </c>
       <c r="K157" t="n">
         <v>31.32</v>
@@ -9278,7 +9278,7 @@
         <v>148.96</v>
       </c>
       <c r="D158" t="n">
-        <v>34.4</v>
+        <v>47.8</v>
       </c>
       <c r="E158" t="n">
         <v>0.4</v>
@@ -9296,7 +9296,7 @@
         <v>0</v>
       </c>
       <c r="J158" t="n">
-        <v>-168.3761286744291</v>
+        <v>-3290.145504699991</v>
       </c>
       <c r="K158" t="n">
         <v>31.7</v>
@@ -9334,7 +9334,7 @@
         <v>148.96</v>
       </c>
       <c r="D159" t="n">
-        <v>17.1</v>
+        <v>47.8</v>
       </c>
       <c r="E159" t="n">
         <v>0.4</v>
@@ -9352,7 +9352,7 @@
         <v>0</v>
       </c>
       <c r="J159" t="n">
-        <v>-161.4560080000001</v>
+        <v>-2970.556903276376</v>
       </c>
       <c r="K159" t="n">
         <v>31.59999</v>
@@ -9408,7 +9408,7 @@
         <v>0</v>
       </c>
       <c r="J160" t="n">
-        <v>-129.0213858541596</v>
+        <v>-2233.527723940623</v>
       </c>
       <c r="K160" t="n">
         <v>31.7</v>
@@ -9455,16 +9455,16 @@
         <v>47.8</v>
       </c>
       <c r="G161" t="n">
-        <v>0</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H161" t="n">
         <v>0</v>
       </c>
       <c r="I161" t="n">
-        <v>6.124</v>
+        <v>6.12399999999998</v>
       </c>
       <c r="J161" t="n">
-        <v>1125.644595506748</v>
+        <v>-2105.725286593471</v>
       </c>
       <c r="K161" t="n">
         <v>31.26</v>
@@ -9517,10 +9517,10 @@
         <v>0</v>
       </c>
       <c r="I162" t="n">
-        <v>0</v>
+        <v>6.12399999999998</v>
       </c>
       <c r="J162" t="n">
-        <v>1171.560018957533</v>
+        <v>-1174.308392180928</v>
       </c>
       <c r="K162" t="n">
         <v>31.41</v>
@@ -9564,19 +9564,19 @@
         <v>0.4</v>
       </c>
       <c r="F163" t="n">
-        <v>7.4</v>
+        <v>32.1</v>
       </c>
       <c r="G163" t="n">
-        <v>0</v>
+        <v>7.836999999999993</v>
       </c>
       <c r="H163" t="n">
-        <v>40.40000000000001</v>
+        <v>15.7</v>
       </c>
       <c r="I163" t="n">
-        <v>0</v>
+        <v>6.123999999999981</v>
       </c>
       <c r="J163" t="n">
-        <v>310.0393012748883</v>
+        <v>-345.2580684900023</v>
       </c>
       <c r="K163" t="n">
         <v>31.4</v>
@@ -9629,10 +9629,10 @@
         <v>0</v>
       </c>
       <c r="I164" t="n">
-        <v>6.659</v>
+        <v>8.423</v>
       </c>
       <c r="J164" t="n">
-        <v>2126.489321276863</v>
+        <v>1663.248620879348</v>
       </c>
       <c r="K164" t="n">
         <v>31.1</v>
@@ -9688,7 +9688,7 @@
         <v>8.423</v>
       </c>
       <c r="J165" t="n">
-        <v>2095.599301835973</v>
+        <v>2092.477616577621</v>
       </c>
       <c r="K165" t="n">
         <v>30.75</v>
@@ -9729,7 +9729,7 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>0.1299999999996544</v>
+        <v>0.27</v>
       </c>
       <c r="F166" t="n">
         <v>47.8</v>
@@ -9744,7 +9744,7 @@
         <v>8.423</v>
       </c>
       <c r="J166" t="n">
-        <v>2069.85851800461</v>
+        <v>2069.858518004612</v>
       </c>
       <c r="K166" t="n">
         <v>30.469999</v>
@@ -9788,19 +9788,19 @@
         <v>0.13</v>
       </c>
       <c r="F167" t="n">
-        <v>47.8</v>
+        <v>19.2</v>
       </c>
       <c r="G167" t="n">
         <v>10.47399999999999</v>
       </c>
       <c r="H167" t="n">
-        <v>0</v>
+        <v>28.6</v>
       </c>
       <c r="I167" t="n">
-        <v>13.913</v>
+        <v>9.842999999999904</v>
       </c>
       <c r="J167" t="n">
-        <v>1863.80694760508</v>
+        <v>563.5800463289191</v>
       </c>
       <c r="K167" t="n">
         <v>30.1</v>
@@ -9853,7 +9853,7 @@
         <v>0</v>
       </c>
       <c r="I168" t="n">
-        <v>14.924</v>
+        <v>13.582</v>
       </c>
       <c r="J168" t="n">
         <v>1790.430491733054</v>
@@ -9909,10 +9909,10 @@
         <v>0</v>
       </c>
       <c r="I169" t="n">
-        <v>26.37</v>
+        <v>25.45200000000001</v>
       </c>
       <c r="J169" t="n">
-        <v>1227.356719147881</v>
+        <v>1227.972070724571</v>
       </c>
       <c r="K169" t="n">
         <v>24.99</v>

</xml_diff>